<commit_message>
Based on push to refs/heads/master by rdswift
</commit_message>
<xml_diff>
--- a/downloads/MusicBrainz_Picard_Tag_Map.xlsx
+++ b/downloads/MusicBrainz_Picard_Tag_Map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="550">
   <si>
     <t>MusicBrainz Picard Tag Mapping</t>
   </si>
@@ -421,6 +421,24 @@
     <t>ICOP</t>
   </si>
   <si>
+    <t>Director</t>
+  </si>
+  <si>
+    <t>director</t>
+  </si>
+  <si>
+    <t>TXXX:DIRECTOR</t>
+  </si>
+  <si>
+    <t>DIRECTOR</t>
+  </si>
+  <si>
+    <t>©dir [9]</t>
+  </si>
+  <si>
+    <t>WM/Director</t>
+  </si>
+  <si>
     <t>Disc Number</t>
   </si>
   <si>
@@ -1656,6 +1674,9 @@
   </si>
   <si>
     <t>8.  With "Save iTunes compatible grouping and work" (since Picard&gt;=2.1.0)</t>
+  </si>
+  <si>
+    <t>9.  From iTunes Metadata Format Specification</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2073,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H103"/>
+  <dimension ref="A1:H105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
@@ -2638,13 +2659,13 @@
         <v>137</v>
       </c>
       <c r="E24" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>15</v>
@@ -2652,25 +2673,25 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>147</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>15</v>
@@ -2678,54 +2699,54 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="G26" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="H26" s="4" t="s">
-        <v>155</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="G27" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2742,108 +2763,108 @@
         <v>165</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>166</v>
+        <v>15</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>167</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D29" s="4" t="s">
-        <v>15</v>
+        <v>171</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>15</v>
+        <v>168</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>172</v>
+        <v>15</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>177</v>
+        <v>15</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>178</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B31" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="C31" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="F31" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="G31" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="H31" s="4" t="s">
         <v>184</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>189</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>189</v>
@@ -2869,16 +2890,16 @@
         <v>194</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>15</v>
@@ -2886,19 +2907,19 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="3" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>200</v>
-      </c>
       <c r="E34" s="4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>201</v>
@@ -2907,56 +2928,56 @@
         <v>202</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>203</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="F35" s="4" t="s">
+      <c r="G35" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="H35" s="4" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>214</v>
+        <v>15</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>15</v>
@@ -2976,13 +2997,13 @@
         <v>218</v>
       </c>
       <c r="E37" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>221</v>
       </c>
       <c r="H37" s="4" t="s">
         <v>15</v>
@@ -2990,19 +3011,19 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>222</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>226</v>
@@ -3011,50 +3032,50 @@
         <v>227</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>228</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="G39" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="H39" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B40" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="C40" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>236</v>
       </c>
       <c r="F40" s="4" t="s">
         <v>240</v>
@@ -3080,13 +3101,13 @@
         <v>245</v>
       </c>
       <c r="E41" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="G41" s="4" t="s">
         <v>247</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>248</v>
       </c>
       <c r="H41" s="4" t="s">
         <v>15</v>
@@ -3094,16 +3115,16 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B42" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>252</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>252</v>
@@ -3112,7 +3133,7 @@
         <v>253</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>15</v>
+        <v>254</v>
       </c>
       <c r="H42" s="4" t="s">
         <v>15</v>
@@ -3120,22 +3141,22 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="3" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="G43" s="4" t="s">
         <v>15</v>
@@ -3146,22 +3167,22 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="3" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="G44" s="4" t="s">
         <v>15</v>
@@ -3172,25 +3193,25 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="3" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>268</v>
+        <v>15</v>
       </c>
       <c r="H45" s="4" t="s">
         <v>15</v>
@@ -3236,7 +3257,7 @@
         <v>278</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>15</v>
+        <v>278</v>
       </c>
       <c r="F47" s="4" t="s">
         <v>279</v>
@@ -3288,7 +3309,7 @@
         <v>290</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>290</v>
+        <v>15</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>291</v>
@@ -3470,13 +3491,13 @@
         <v>332</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>15</v>
+        <v>332</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>333</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>15</v>
+        <v>334</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>15</v>
@@ -3484,25 +3505,25 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="3" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>337</v>
+        <v>15</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>339</v>
+        <v>15</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>15</v>
@@ -3519,16 +3540,16 @@
         <v>342</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>15</v>
+        <v>343</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>15</v>
+        <v>343</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>15</v>
+        <v>344</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H58" s="4" t="s">
         <v>15</v>
@@ -3536,25 +3557,25 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="3" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>347</v>
+        <v>15</v>
       </c>
       <c r="F59" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="H59" s="4" t="s">
         <v>15</v>
@@ -3562,25 +3583,25 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>352</v>
+        <v>15</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="F60" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="H60" s="4" t="s">
         <v>15</v>
@@ -3588,25 +3609,25 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="3" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>15</v>
+        <v>358</v>
       </c>
       <c r="F61" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>15</v>
@@ -3614,25 +3635,25 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="3" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>15</v>
+        <v>362</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>361</v>
+        <v>15</v>
       </c>
       <c r="F62" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="H62" s="4" t="s">
         <v>15</v>
@@ -3640,16 +3661,16 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>365</v>
+        <v>15</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>367</v>
@@ -3658,7 +3679,7 @@
         <v>15</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>15</v>
+        <v>368</v>
       </c>
       <c r="H63" s="4" t="s">
         <v>15</v>
@@ -3666,22 +3687,22 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>15</v>
+        <v>371</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>15</v>
+        <v>372</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>15</v>
+        <v>373</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>370</v>
+        <v>15</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>15</v>
@@ -3692,10 +3713,10 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="3" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>15</v>
@@ -3707,7 +3728,7 @@
         <v>15</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>15</v>
@@ -3718,77 +3739,77 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="3" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>376</v>
+        <v>15</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>377</v>
+        <v>15</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>374</v>
+        <v>15</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>379</v>
+        <v>15</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>380</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>381</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C67" s="4" t="s">
+      <c r="D67" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D67" s="4" t="s">
+      <c r="E67" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="F67" s="4" t="s">
         <v>384</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>385</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>15</v>
+        <v>386</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="3" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>390</v>
+        <v>15</v>
       </c>
       <c r="F68" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" s="4" t="s">
         <v>391</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>392</v>
       </c>
       <c r="H68" s="4" t="s">
         <v>15</v>
@@ -3796,16 +3817,16 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="C69" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="D69" s="4" t="s">
         <v>395</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>396</v>
       </c>
       <c r="E69" s="4" t="s">
         <v>396</v>
@@ -3817,82 +3838,82 @@
         <v>398</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>399</v>
+        <v>15</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B70" s="4" t="s">
         <v>400</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="C70" s="4" t="s">
         <v>401</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="D70" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="E70" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="F70" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="G70" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="F70" s="4" t="s">
+      <c r="H70" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="G70" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="H70" s="4" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="D71" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="C71" s="4" t="s">
+      <c r="E71" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="D71" s="4" t="s">
+      <c r="F71" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="E71" s="4" t="s">
+      <c r="G71" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="F71" s="4" t="s">
+      <c r="H71" s="4" t="s">
         <v>413</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>416</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="D72" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="D72" s="4" t="s">
+      <c r="E72" s="4" t="s">
         <v>418</v>
       </c>
-      <c r="E72" s="4" t="s">
+      <c r="F72" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F72" s="4" t="s">
+      <c r="G72" s="4" t="s">
         <v>420</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>421</v>
       </c>
       <c r="H72" s="4" t="s">
         <v>15</v>
@@ -3900,25 +3921,25 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B73" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="C73" s="4" t="s">
         <v>423</v>
       </c>
-      <c r="C73" s="4" t="s">
+      <c r="D73" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="D73" s="4" t="s">
+      <c r="E73" s="4" t="s">
         <v>425</v>
       </c>
-      <c r="E73" s="4" t="s">
+      <c r="F73" s="4" t="s">
         <v>426</v>
       </c>
-      <c r="F73" s="4" t="s">
+      <c r="G73" s="4" t="s">
         <v>427</v>
-      </c>
-      <c r="G73" s="4" t="s">
-        <v>428</v>
       </c>
       <c r="H73" s="4" t="s">
         <v>15</v>
@@ -3926,16 +3947,16 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>429</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>430</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="D74" s="4" t="s">
         <v>431</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>432</v>
       </c>
       <c r="E74" s="4" t="s">
         <v>432</v>
@@ -3944,7 +3965,7 @@
         <v>433</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>15</v>
@@ -3952,25 +3973,25 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" s="3" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="F75" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="G75" s="4" t="s">
         <v>438</v>
-      </c>
-      <c r="G75" s="4" t="s">
-        <v>437</v>
       </c>
       <c r="H75" s="4" t="s">
         <v>15</v>
@@ -3978,25 +3999,25 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" s="3" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="F76" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="G76" s="4" t="s">
         <v>443</v>
-      </c>
-      <c r="G76" s="4" t="s">
-        <v>442</v>
       </c>
       <c r="H76" s="4" t="s">
         <v>15</v>
@@ -4004,25 +4025,25 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="F77" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="G77" s="4" t="s">
         <v>448</v>
-      </c>
-      <c r="G77" s="4" t="s">
-        <v>447</v>
       </c>
       <c r="H77" s="4" t="s">
         <v>15</v>
@@ -4030,25 +4051,25 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F78" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="G78" s="4" t="s">
         <v>453</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>452</v>
       </c>
       <c r="H78" s="4" t="s">
         <v>15</v>
@@ -4056,25 +4077,25 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="3" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F79" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="G79" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="G79" s="4" t="s">
-        <v>457</v>
       </c>
       <c r="H79" s="4" t="s">
         <v>15</v>
@@ -4082,25 +4103,25 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="3" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F80" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="G80" s="4" t="s">
         <v>463</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>15</v>
@@ -4108,25 +4129,25 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" s="3" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="F81" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="G81" s="4" t="s">
         <v>468</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>469</v>
       </c>
       <c r="H81" s="4" t="s">
         <v>15</v>
@@ -4140,19 +4161,19 @@
         <v>471</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>15</v>
+        <v>472</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>15</v>
+        <v>473</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>15</v>
+        <v>470</v>
       </c>
       <c r="F82" s="4" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="G82" s="4" t="s">
-        <v>15</v>
+        <v>475</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>15</v>
@@ -4160,10 +4181,10 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="3" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>15</v>
@@ -4175,7 +4196,7 @@
         <v>15</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>15</v>
@@ -4186,22 +4207,22 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="3" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>478</v>
+        <v>15</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>479</v>
+        <v>15</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>479</v>
+        <v>15</v>
       </c>
       <c r="F84" s="4" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>15</v>
@@ -4212,16 +4233,16 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="3" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E85" s="4" t="s">
         <v>485</v>
@@ -4230,7 +4251,7 @@
         <v>486</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>487</v>
+        <v>15</v>
       </c>
       <c r="H85" s="4" t="s">
         <v>15</v>
@@ -4238,25 +4259,25 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="B86" s="4" t="s">
         <v>488</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="C86" s="4" t="s">
         <v>489</v>
-      </c>
-      <c r="C86" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="D86" s="4" t="s">
         <v>490</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>138</v>
+        <v>491</v>
       </c>
       <c r="F86" s="4" t="s">
-        <v>139</v>
+        <v>492</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="H86" s="4" t="s">
         <v>15</v>
@@ -4264,25 +4285,25 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>494</v>
+        <v>142</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>496</v>
+        <v>144</v>
       </c>
       <c r="F87" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G87" s="4" t="s">
         <v>497</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>15</v>
@@ -4296,62 +4317,62 @@
         <v>499</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="G88" s="4" t="s">
-        <v>501</v>
+        <v>15</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>502</v>
+        <v>15</v>
       </c>
     </row>
     <row r="89" spans="1:8">
       <c r="A89" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="D89" s="4" t="s">
         <v>506</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G89" s="4" t="s">
         <v>507</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="90" spans="1:8">
       <c r="A90" s="3" t="s">
+        <v>509</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="D90" s="4" t="s">
         <v>512</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>513</v>
       </c>
       <c r="E90" s="4" t="s">
         <v>513</v>
@@ -4360,10 +4381,10 @@
         <v>514</v>
       </c>
       <c r="G90" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="H90" s="4" t="s">
         <v>515</v>
-      </c>
-      <c r="H90" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -4380,10 +4401,10 @@
         <v>519</v>
       </c>
       <c r="E91" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="F91" s="4" t="s">
         <v>520</v>
-      </c>
-      <c r="F91" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="G91" s="4" t="s">
         <v>521</v>
@@ -4406,10 +4427,10 @@
         <v>525</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="F92" s="4" t="s">
-        <v>526</v>
+        <v>15</v>
       </c>
       <c r="G92" s="4" t="s">
         <v>527</v>
@@ -4432,61 +4453,92 @@
         <v>531</v>
       </c>
       <c r="E93" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="F93" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="F93" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="G93" s="4" t="s">
-        <v>15</v>
+        <v>533</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="B95" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8">
+      <c r="A94" s="3" t="s">
         <v>534</v>
       </c>
+      <c r="B94" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>538</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>539</v>
+      </c>
     </row>
     <row r="96" spans="1:8">
-      <c r="B96" t="s">
-        <v>535</v>
+      <c r="B96" s="5" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
     </row>
     <row r="98" spans="2:2">
       <c r="B98" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
     </row>
     <row r="99" spans="2:2">
       <c r="B99" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
     </row>
     <row r="100" spans="2:2">
       <c r="B100" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
     </row>
     <row r="101" spans="2:2">
       <c r="B101" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
     </row>
     <row r="102" spans="2:2">
       <c r="B102" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
     </row>
     <row r="103" spans="2:2">
       <c r="B103" t="s">
-        <v>542</v>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2">
+      <c r="B104" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2">
+      <c r="B105" t="s">
+        <v>549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>